<commit_message>
Some changes in HW4 grading program grade matrix.
</commit_message>
<xml_diff>
--- a/auto_grading/hw3_grading/BeforeGrading.xlsx
+++ b/auto_grading/hw3_grading/BeforeGrading.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="555" yWindow="555" windowWidth="20610" windowHeight="11640" tabRatio="500" activeTab="1"/>
@@ -10,10 +10,7 @@
     <sheet name="BeforeGrading.csv" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">BeforeGrading.csv!$A$1:$AE$60</definedName>
-  </definedNames>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -23,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="152">
   <si>
     <t>Uni</t>
   </si>
@@ -467,6 +464,22 @@
   </si>
   <si>
     <t>tg2342</t>
+  </si>
+  <si>
+    <t>didn't finish</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>some bugs, didn't converge.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Estep wrong,some bugs, didn't converge</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>didn't add bias in previous questions</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -913,13 +926,16 @@
   </sheetPr>
   <dimension ref="A1:AE123"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="555" topLeftCell="A37" activePane="bottomLeft"/>
-      <selection activeCell="A30" sqref="A30"/>
-      <selection pane="bottomLeft" activeCell="AE65" sqref="AE65:AE123"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="555" topLeftCell="A7" activePane="bottomLeft"/>
+      <selection activeCell="AC1" sqref="AC1"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="14.25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:31">
       <c r="A1" t="s">
@@ -4105,7 +4121,7 @@
         <v>1</v>
       </c>
       <c r="AE34">
-        <f t="shared" ref="AE34:AE65" si="1">SUM(B34:AD34)/30</f>
+        <f t="shared" ref="AE34:AE60" si="1">SUM(B34:AD34)/30</f>
         <v>0.1</v>
       </c>
     </row>
@@ -14027,10 +14043,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -14163,7 +14179,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>105</v>
       </c>
@@ -14171,7 +14187,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>106</v>
       </c>
@@ -14179,7 +14195,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>107</v>
       </c>
@@ -14187,7 +14203,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>108</v>
       </c>
@@ -14195,7 +14211,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>109</v>
       </c>
@@ -14203,7 +14219,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>110</v>
       </c>
@@ -14211,15 +14227,21 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:2" s="2" customFormat="1">
+    <row r="23" spans="1:4" s="2" customFormat="1">
       <c r="A23" s="2" t="s">
         <v>111</v>
       </c>
       <c r="B23" s="2">
         <v>95</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" s="2">
+        <v>15</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>112</v>
       </c>
@@ -14227,7 +14249,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>113</v>
       </c>
@@ -14235,7 +14257,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>114</v>
       </c>
@@ -14243,7 +14265,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>115</v>
       </c>
@@ -14251,7 +14273,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>116</v>
       </c>
@@ -14259,7 +14281,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>117</v>
       </c>
@@ -14267,7 +14289,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>118</v>
       </c>
@@ -14275,7 +14297,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>119</v>
       </c>
@@ -14283,7 +14305,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>120</v>
       </c>
@@ -14291,7 +14313,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>121</v>
       </c>
@@ -14299,7 +14321,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>122</v>
       </c>
@@ -14307,7 +14329,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>123</v>
       </c>
@@ -14315,7 +14337,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>124</v>
       </c>
@@ -14323,15 +14345,21 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:2" s="2" customFormat="1">
+    <row r="37" spans="1:4" s="2" customFormat="1">
       <c r="A37" s="2" t="s">
         <v>125</v>
       </c>
       <c r="B37" s="2">
         <v>85</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37" s="2">
+        <v>10</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>126</v>
       </c>
@@ -14339,7 +14367,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>127</v>
       </c>
@@ -14347,7 +14375,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>128</v>
       </c>
@@ -14355,7 +14383,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>129</v>
       </c>
@@ -14363,7 +14391,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>130</v>
       </c>
@@ -14371,7 +14399,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>131</v>
       </c>
@@ -14379,7 +14407,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>132</v>
       </c>
@@ -14387,7 +14415,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>133</v>
       </c>
@@ -14395,7 +14423,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>134</v>
       </c>
@@ -14403,7 +14431,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>135</v>
       </c>
@@ -14411,15 +14439,21 @@
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:2" s="2" customFormat="1">
+    <row r="48" spans="1:4" s="2" customFormat="1">
       <c r="A48" s="2" t="s">
         <v>136</v>
       </c>
       <c r="B48" s="2">
         <v>75</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="C48" s="2">
+        <v>24</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>137</v>
       </c>
@@ -14427,15 +14461,21 @@
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:2" s="2" customFormat="1">
+    <row r="50" spans="1:4" s="2" customFormat="1">
       <c r="A50" s="2" t="s">
         <v>138</v>
       </c>
       <c r="B50" s="2">
         <v>66</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="C50" s="2">
+        <v>15</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>139</v>
       </c>
@@ -14443,7 +14483,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>140</v>
       </c>
@@ -14451,7 +14491,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>141</v>
       </c>
@@ -14459,7 +14499,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>142</v>
       </c>
@@ -14467,15 +14507,21 @@
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:2" s="2" customFormat="1">
+    <row r="55" spans="1:4" s="2" customFormat="1">
       <c r="A55" s="2" t="s">
         <v>143</v>
       </c>
       <c r="B55" s="2">
         <v>45</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="C55" s="2">
+        <v>0</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>144</v>
       </c>
@@ -14483,7 +14529,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>145</v>
       </c>
@@ -14491,7 +14537,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>146</v>
       </c>
@@ -14499,7 +14545,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>147</v>
       </c>

</xml_diff>